<commit_message>
illustrative examples scripts and figures improvements
</commit_message>
<xml_diff>
--- a/otherData/BCC_Data.xlsx
+++ b/otherData/BCC_Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\osinf\Dropbox\Software\Performance_AJ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\GitHub\pysigmap\otherData\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF4A780-391C-4682-B6EA-DB5C0A59FE68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8808"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -358,19 +359,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.6" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="13.2" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="6.9453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.9453125" style="1"/>
+    <col min="1" max="2" width="7" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -381,7 +384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -392,7 +395,7 @@
         <v>0.77518951641226796</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>6.18</v>
       </c>
@@ -403,7 +406,7 @@
         <v>0.75974536761948119</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>12.36</v>
       </c>
@@ -414,7 +417,7 @@
         <v>0.74678648414967164</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>24.81</v>
       </c>
@@ -425,7 +428,7 @@
         <v>0.73045474059867876</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>49.52</v>
       </c>
@@ -436,7 +439,7 @@
         <v>0.70915246640173157</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>99.05</v>
       </c>
@@ -447,7 +450,7 @@
         <v>0.68465485107524227</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>198.19</v>
       </c>
@@ -458,7 +461,7 @@
         <v>0.65638495802637697</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>396.38</v>
       </c>
@@ -469,7 +472,7 @@
         <v>0.61684261154829367</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>792.77</v>
       </c>
@@ -480,7 +483,7 @@
         <v>0.57388302525111679</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>1585.43</v>
       </c>
@@ -491,7 +494,7 @@
         <v>0.51277212614862444</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>792.77</v>
       </c>
@@ -502,7 +505,7 @@
         <v>0.51991726395218385</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>396.38</v>
       </c>
@@ -513,7 +516,7 @@
         <v>0.5321660716154285</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>198.19</v>
       </c>
@@ -524,7 +527,7 @@
         <v>0.54832029621478018</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>99.05</v>
       </c>
@@ -535,7 +538,7 @@
         <v>0.56607219137890286</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>49.52</v>
       </c>
@@ -546,7 +549,7 @@
         <v>0.58613183291436144</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>99.05</v>
       </c>
@@ -557,7 +560,7 @@
         <v>0.5797411506552772</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>198.19</v>
       </c>
@@ -568,7 +571,7 @@
         <v>0.56695978613710896</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>396.38</v>
       </c>
@@ -579,7 +582,7 @@
         <v>0.54867533411806257</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>792.77</v>
       </c>
@@ -590,7 +593,7 @@
         <v>0.52861569258260399</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>1585.43</v>
       </c>
@@ -601,7 +604,7 @@
         <v>0.49985762241672521</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>3170.87</v>
       </c>
@@ -612,7 +615,7 @@
         <v>0.441808925230044</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>6341.83</v>
       </c>
@@ -623,7 +626,7 @@
         <v>0.37577187521950767</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>3170.87</v>
       </c>
@@ -634,7 +637,7 @@
         <v>0.37878969739740859</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>1585.43</v>
       </c>
@@ -645,7 +648,7 @@
         <v>0.39139354296393564</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>792.77</v>
       </c>
@@ -656,7 +659,7 @@
         <v>0.40719272966000492</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>396.38</v>
       </c>
@@ -667,7 +670,7 @@
         <v>0.42600973853397484</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>198.19</v>
       </c>

</xml_diff>